<commit_message>
Aggiornato Diario + Commenti aggiunti al codice
</commit_message>
<xml_diff>
--- a/9_Cose esterne/Excel_Gannt-Lavori-svolti-e-in-corso.xlsx
+++ b/9_Cose esterne/Excel_Gannt-Lavori-svolti-e-in-corso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\I3BB - 23-24\!PROGETTI\Git\FindTheWord\9_Cose esterne\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC306A92-9CCA-4A71-ABEB-B9D6A85DBAE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3E7461-FE91-4013-86BA-E7CD8B9B8610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{129BD50E-E7E7-4711-8371-76A95D9454F9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>Modalità attività</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>0.96 g</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Design</t>
   </si>
   <si>
     <t xml:space="preserve">      Design delle classi</t>
@@ -217,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +248,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -325,6 +346,21 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -333,6 +369,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF00FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -641,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{893D27E1-B168-4055-AE29-7FF0932B991E}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +719,7 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -773,7 +814,7 @@
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -791,20 +832,20 @@
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8">
         <v>45184.347222222219</v>
       </c>
-      <c r="E8" s="4">
-        <v>45191.427083333336</v>
+      <c r="E8" s="8">
+        <v>45184.65625</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="1"/>
@@ -814,137 +855,137 @@
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="8">
         <v>45184.347222222219</v>
       </c>
       <c r="E9" s="8">
-        <v>45184.65625</v>
+        <v>45184.440972222219</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D10" s="8">
-        <v>45184.347222222219</v>
+        <v>45191.333333333336</v>
       </c>
       <c r="E10" s="8">
-        <v>45184.440972222219</v>
+        <v>45191.427083333336</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="4">
         <v>45191.333333333336</v>
       </c>
-      <c r="E11" s="8">
-        <v>45191.427083333336</v>
-      </c>
-      <c r="F11" s="5"/>
+      <c r="E11" s="4">
+        <v>45254.368055555555</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4">
+      <c r="C12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="8">
         <v>45191.333333333336</v>
       </c>
-      <c r="E12" s="4">
-        <v>45254.368055555555</v>
-      </c>
-      <c r="F12" s="3">
-        <v>6</v>
-      </c>
+      <c r="E12" s="8">
+        <v>45191.354166666664</v>
+      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D13" s="8">
-        <v>45191.333333333336</v>
+        <v>45191.354166666664</v>
       </c>
       <c r="E13" s="8">
-        <v>45191.354166666664</v>
+        <v>45198.354166666664</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="8">
-        <v>45191.354166666664</v>
-      </c>
-      <c r="E14" s="8">
-        <v>45198.354166666664</v>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4">
+        <v>45198.368055555555</v>
+      </c>
+      <c r="E14" s="4">
+        <v>45240.368055555555</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="3" t="s">
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="4">
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="8">
         <v>45198.368055555555</v>
       </c>
-      <c r="E15" s="4">
-        <v>45240.368055555555</v>
+      <c r="E15" s="8">
+        <v>45205.368055555555</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>9</v>
       </c>
@@ -952,18 +993,18 @@
         <v>32</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="8">
-        <v>45198.368055555555</v>
+        <v>45205.368055555555</v>
       </c>
       <c r="E16" s="8">
-        <v>45205.368055555555</v>
+        <v>45205.461805555555</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>9</v>
       </c>
@@ -971,13 +1012,13 @@
         <v>33</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D17" s="8">
-        <v>45205.368055555555</v>
+        <v>45205.461805555555</v>
       </c>
       <c r="E17" s="8">
-        <v>45205.461805555555</v>
+        <v>45212.461805555555</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="1"/>
@@ -986,17 +1027,17 @@
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D18" s="8">
-        <v>45205.461805555555</v>
+        <v>45212.461805555555</v>
       </c>
       <c r="E18" s="8">
-        <v>45212.461805555555</v>
+        <v>45219.583333333336</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="1"/>
@@ -1005,181 +1046,181 @@
       <c r="A19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="D19" s="8">
-        <v>45212.461805555555</v>
+        <v>45219.59375</v>
       </c>
       <c r="E19" s="8">
-        <v>45219.583333333336</v>
+        <v>45240.368055555555</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="14" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D20" s="8">
-        <v>45219.59375</v>
+        <v>45205.368055555555</v>
       </c>
       <c r="E20" s="8">
-        <v>45240.368055555555</v>
+        <v>45205.388888888891</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8">
-        <v>45205.368055555555</v>
-      </c>
-      <c r="E21" s="8">
-        <v>45205.388888888891</v>
-      </c>
-      <c r="F21" s="5"/>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4">
+        <v>45240.368055555555</v>
+      </c>
+      <c r="E21" s="4">
+        <v>45254.368055555555</v>
+      </c>
+      <c r="F21" s="3">
+        <v>14</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="C22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="8">
         <v>45240.368055555555</v>
       </c>
-      <c r="E22" s="4">
-        <v>45254.368055555555</v>
-      </c>
-      <c r="F22" s="3">
-        <v>14</v>
-      </c>
+      <c r="E22" s="8">
+        <v>45240.583333333336</v>
+      </c>
+      <c r="F22" s="5"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="D23" s="8">
-        <v>45240.368055555555</v>
+        <v>45240.59375</v>
       </c>
       <c r="E23" s="8">
-        <v>45240.583333333336</v>
+        <v>45247.461805555555</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D24" s="8">
-        <v>45240.59375</v>
+        <v>45247.461805555555</v>
       </c>
       <c r="E24" s="8">
-        <v>45247.461805555555</v>
+        <v>45247.583333333336</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" s="8">
-        <v>45247.461805555555</v>
+        <v>45247.59375</v>
       </c>
       <c r="E25" s="8">
-        <v>45247.583333333336</v>
+        <v>45254.368055555555</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="D26" s="8">
-        <v>45247.59375</v>
+        <v>45254.368055555555</v>
       </c>
       <c r="E26" s="8">
-        <v>45254.368055555555</v>
+        <v>45254.635416666664</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="8">
-        <v>45254.368055555555</v>
-      </c>
-      <c r="E27" s="8">
-        <v>45254.635416666664</v>
-      </c>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="8">
+        <v>45170.333333333336</v>
+      </c>
+      <c r="E28" s="8">
+        <v>45261.708333333336</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="1"/>
     </row>
@@ -1187,11 +1228,11 @@
       <c r="A29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="D29" s="8">
         <v>45170.333333333336</v>
@@ -1202,52 +1243,33 @@
       <c r="F29" s="5"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="8">
-        <v>45170.333333333336</v>
-      </c>
-      <c r="E30" s="8">
-        <v>45261.708333333336</v>
-      </c>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="8">
+        <v>45261.347222222219</v>
+      </c>
+      <c r="E31" s="8">
+        <v>45261.347222222219</v>
+      </c>
       <c r="F31" s="5"/>
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="8">
-        <v>45261.347222222219</v>
-      </c>
-      <c r="E32" s="8">
-        <v>45261.347222222219</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>